<commit_message>
feat: update Excel template file
</commit_message>
<xml_diff>
--- a/client/public/template-questions.xlsx
+++ b/client/public/template-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2495BE-2BCA-4976-9881-F927E648410E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D06F44-76D1-420E-B63B-F24E96956C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Câu hỏi</t>
   </si>
@@ -151,6 +151,24 @@
   <si>
     <t>Tác phẩm "Crime and Punishment" được viết bởi ai?</t>
   </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lưu ý: kết thúc bộ đề bằng từ khóa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>END</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -207,12 +225,6 @@
       <name val="Tahoma"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="11"/>
@@ -249,6 +261,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -390,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -425,40 +444,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,7 +693,7 @@
   <dimension ref="A1:AB1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -733,8 +749,8 @@
       <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17">
         <v>2</v>
       </c>
       <c r="D2" s="6"/>
@@ -764,9 +780,9 @@
       <c r="AB2" s="8"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
@@ -798,9 +814,9 @@
       <c r="AB3" s="8"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
@@ -830,9 +846,9 @@
       <c r="AB4" s="8"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -860,13 +876,13 @@
       <c r="AB5" s="8"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -898,9 +914,9 @@
       <c r="AB6" s="8"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
@@ -932,9 +948,9 @@
       <c r="AB7" s="8"/>
     </row>
     <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
@@ -966,9 +982,9 @@
       <c r="AB8" s="8"/>
     </row>
     <row r="9" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
@@ -996,11 +1012,11 @@
       <c r="AB9" s="8"/>
     </row>
     <row r="10" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17">
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1032,9 +1048,9 @@
       <c r="AB10" s="8"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1066,9 +1082,9 @@
       <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
@@ -1098,9 +1114,9 @@
       <c r="AB12" s="8"/>
     </row>
     <row r="13" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="6" t="s">
         <v>15</v>
       </c>
@@ -1130,11 +1146,11 @@
       <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17">
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1168,9 +1184,9 @@
       <c r="AB14" s="8"/>
     </row>
     <row r="15" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="6" t="s">
         <v>25</v>
       </c>
@@ -1200,9 +1216,9 @@
       <c r="AB15" s="8"/>
     </row>
     <row r="16" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
@@ -1232,9 +1248,9 @@
       <c r="AB16" s="8"/>
     </row>
     <row r="17" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
@@ -1264,11 +1280,11 @@
       <c r="AB17" s="8"/>
     </row>
     <row r="18" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1300,9 +1316,9 @@
       <c r="AB18" s="8"/>
     </row>
     <row r="19" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1334,9 +1350,9 @@
       <c r="AB19" s="8"/>
     </row>
     <row r="20" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="6" t="s">
         <v>23</v>
       </c>
@@ -1366,11 +1382,11 @@
       <c r="AB20" s="8"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="15"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -1396,11 +1412,13 @@
       <c r="AB21" s="8"/>
     </row>
     <row r="22" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="A22" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -1486,7 +1504,7 @@
       <c r="AB24" s="8"/>
     </row>
     <row r="25" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="8"/>
@@ -1518,7 +1536,7 @@
       <c r="AB25" s="8"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8"/>
@@ -1550,7 +1568,9 @@
       <c r="AB26" s="8"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
+      <c r="A27" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1732,7 +1752,7 @@
       <c r="AB32" s="8"/>
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -30893,11 +30913,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
@@ -30910,6 +30925,11 @@
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>